<commit_message>
fixed category classifier for better results
</commit_message>
<xml_diff>
--- a/static/sysfiles/download/results.xlsx
+++ b/static/sysfiles/download/results.xlsx
@@ -2025,7 +2025,7 @@
         <v>119</v>
       </c>
       <c r="I44" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -2083,7 +2083,7 @@
         <v>119</v>
       </c>
       <c r="I46" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -3127,7 +3127,7 @@
         <v>118</v>
       </c>
       <c r="I82" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -3156,7 +3156,7 @@
         <v>118</v>
       </c>
       <c r="I83" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -3214,7 +3214,7 @@
         <v>118</v>
       </c>
       <c r="I85" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -3301,7 +3301,7 @@
         <v>118</v>
       </c>
       <c r="I88" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="89" spans="1:9">

</xml_diff>